<commit_message>
Fixed typo in CarButtonControl
</commit_message>
<xml_diff>
--- a/portfolio/logs/pr/CarButtonControl_peer_review.xlsx
+++ b/portfolio/logs/pr/CarButtonControl_peer_review.xlsx
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Numbering of states not consistent with team convention</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Requirment 9.1.3 labled as 9.1.2</t>
   </si>
   <si>
     <t>Fixed</t>
@@ -280,8 +286,12 @@
       <c s="7" r="A11">
         <v>2.0</v>
       </c>
-      <c s="9" r="B11"/>
-      <c s="2" r="C11"/>
+      <c t="s" s="8" r="B11">
+        <v>14</v>
+      </c>
+      <c t="s" s="4" r="C11">
+        <v>15</v>
+      </c>
     </row>
     <row customHeight="1" r="12" ht="12.75">
       <c s="7" r="A12">
@@ -381,24 +391,24 @@
     </row>
     <row customHeight="1" r="26" ht="12.75">
       <c t="s" s="2" r="A26">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" s="2" r="B26">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c s="2" r="C26"/>
     </row>
     <row customHeight="1" r="27" ht="12.75">
       <c s="2" r="A27"/>
       <c t="s" s="2" r="B27">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c s="2" r="C27"/>
     </row>
     <row customHeight="1" r="28" ht="12.75">
       <c s="2" r="A28"/>
       <c t="s" s="2" r="B28">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c s="2" r="C28"/>
     </row>

</xml_diff>